<commit_message>
commit 2 dummy nutrient
</commit_message>
<xml_diff>
--- a/nutrients.xlsx
+++ b/nutrients.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jyoth\Desktop\Project Expo\01. Nutri Master\05. Prototype\pdf_upload_website - v0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382E4A57-EDC1-499E-ADB7-8CCC68CB3F7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4875E003-87B3-4593-8F71-0C18D12EE8FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="8743" activeTab="2" xr2:uid="{7978047E-B5C9-4231-8CB2-CE9F13F7E962}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="115">
   <si>
     <t>general_name</t>
   </si>
@@ -340,33 +340,12 @@
     <t>Sunflower Seeds</t>
   </si>
   <si>
-    <t>Nutrient</t>
-  </si>
-  <si>
-    <t>Min_Age</t>
-  </si>
-  <si>
-    <t>Max_Age</t>
-  </si>
-  <si>
-    <t>Gender</t>
-  </si>
-  <si>
-    <t>Activity_Level</t>
-  </si>
-  <si>
-    <t>RDA</t>
-  </si>
-  <si>
     <t>Female</t>
   </si>
   <si>
     <t>Sedentary</t>
   </si>
   <si>
-    <t>18mg</t>
-  </si>
-  <si>
     <t>Moderate</t>
   </si>
   <si>
@@ -376,34 +355,34 @@
     <t>Male</t>
   </si>
   <si>
-    <t>8mg</t>
-  </si>
-  <si>
-    <t>75mg</t>
-  </si>
-  <si>
-    <t>90mg</t>
-  </si>
-  <si>
-    <t>1000mg</t>
-  </si>
-  <si>
-    <t>46g</t>
-  </si>
-  <si>
-    <t>56g</t>
-  </si>
-  <si>
-    <t>1.1g</t>
-  </si>
-  <si>
-    <t>1.6g</t>
-  </si>
-  <si>
-    <t>25g</t>
-  </si>
-  <si>
-    <t>30g</t>
+    <t>min_age</t>
+  </si>
+  <si>
+    <t>max_age</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>activity_level</t>
+  </si>
+  <si>
+    <t>rda_value</t>
+  </si>
+  <si>
+    <t>nutrient_value</t>
+  </si>
+  <si>
+    <t>nutrient_unit</t>
+  </si>
+  <si>
+    <t>mg</t>
+  </si>
+  <si>
+    <t>rda_unit</t>
+  </si>
+  <si>
+    <t>g</t>
   </si>
 </sst>
 </file>
@@ -813,900 +792,1566 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB04BE10-4976-4977-B5EF-3B75D113ED78}">
-  <dimension ref="A1:B111"/>
+  <dimension ref="A1:D111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E118" sqref="E118"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C2">
+        <v>1.5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C3">
+        <v>2.5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C6">
+        <v>5.5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="B7" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C7">
+        <v>0.75</v>
+      </c>
+      <c r="D7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C8">
+        <v>0.9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C9">
+        <v>1.2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>4</v>
       </c>
       <c r="B10" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C10">
+        <v>1.5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>4</v>
       </c>
       <c r="B11" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C11">
+        <v>2.5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>4</v>
       </c>
       <c r="B12" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>4</v>
       </c>
       <c r="B13" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>5</v>
       </c>
       <c r="B14" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C14">
+        <v>5.5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>5</v>
       </c>
       <c r="B15" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C15">
+        <v>0.75</v>
+      </c>
+      <c r="D15" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>5</v>
       </c>
       <c r="B16" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C16">
+        <v>0.9</v>
+      </c>
+      <c r="D16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>5</v>
       </c>
       <c r="B17" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C17">
+        <v>1.2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>5</v>
       </c>
       <c r="B18" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C18">
+        <v>1.5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>7</v>
       </c>
       <c r="B19" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C19">
+        <v>2.5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>7</v>
       </c>
       <c r="B20" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>7</v>
       </c>
       <c r="B21" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>7</v>
       </c>
       <c r="B22" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C22">
+        <v>5.5</v>
+      </c>
+      <c r="D22" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>7</v>
       </c>
       <c r="B23" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C23">
+        <v>0.75</v>
+      </c>
+      <c r="D23" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>8</v>
       </c>
       <c r="B24" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C24">
+        <v>0.9</v>
+      </c>
+      <c r="D24" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>8</v>
       </c>
       <c r="B25" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C25">
+        <v>1.2</v>
+      </c>
+      <c r="D25" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>8</v>
       </c>
       <c r="B26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C26">
+        <v>1.5</v>
+      </c>
+      <c r="D26" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>8</v>
       </c>
       <c r="B27" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C27">
+        <v>2.5</v>
+      </c>
+      <c r="D27" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>8</v>
       </c>
       <c r="B28" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C28">
+        <v>4</v>
+      </c>
+      <c r="D28" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>9</v>
       </c>
       <c r="B29" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C29">
+        <v>3</v>
+      </c>
+      <c r="D29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>9</v>
       </c>
       <c r="B30" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C30">
+        <v>5.5</v>
+      </c>
+      <c r="D30" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>9</v>
       </c>
       <c r="B31" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C31">
+        <v>0.75</v>
+      </c>
+      <c r="D31" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>9</v>
       </c>
       <c r="B32" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C32">
+        <v>0.9</v>
+      </c>
+      <c r="D32" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>9</v>
       </c>
       <c r="B33" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C33">
+        <v>1.2</v>
+      </c>
+      <c r="D33" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>9</v>
       </c>
       <c r="B34" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C34">
+        <v>1.5</v>
+      </c>
+      <c r="D34" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>10</v>
       </c>
       <c r="B35" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C35">
+        <v>2.5</v>
+      </c>
+      <c r="D35" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>10</v>
       </c>
       <c r="B36" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C36">
+        <v>4</v>
+      </c>
+      <c r="D36" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>10</v>
       </c>
       <c r="B37" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>10</v>
       </c>
       <c r="B38" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C38">
+        <v>5.5</v>
+      </c>
+      <c r="D38" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>10</v>
       </c>
       <c r="B39" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C39">
+        <v>0.75</v>
+      </c>
+      <c r="D39" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>13</v>
       </c>
       <c r="B40" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C40">
+        <v>0.9</v>
+      </c>
+      <c r="D40" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>13</v>
       </c>
       <c r="B41" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C41">
+        <v>1.2</v>
+      </c>
+      <c r="D41" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>13</v>
       </c>
       <c r="B42" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C42">
+        <v>1.5</v>
+      </c>
+      <c r="D42" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>13</v>
       </c>
       <c r="B43" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C43">
+        <v>2.5</v>
+      </c>
+      <c r="D43" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
         <v>13</v>
       </c>
       <c r="B44" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C44">
+        <v>4</v>
+      </c>
+      <c r="D44" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
         <v>13</v>
       </c>
       <c r="B45" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
         <v>14</v>
       </c>
       <c r="B46" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C46">
+        <v>5.5</v>
+      </c>
+      <c r="D46" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
         <v>14</v>
       </c>
       <c r="B47" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C47">
+        <v>0.75</v>
+      </c>
+      <c r="D47" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
         <v>14</v>
       </c>
       <c r="B48" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C48">
+        <v>0.9</v>
+      </c>
+      <c r="D48" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
         <v>14</v>
       </c>
       <c r="B49" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C49">
+        <v>1.2</v>
+      </c>
+      <c r="D49" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
         <v>14</v>
       </c>
       <c r="B50" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C50">
+        <v>1.5</v>
+      </c>
+      <c r="D50" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
         <v>15</v>
       </c>
       <c r="B51" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C51">
+        <v>2.5</v>
+      </c>
+      <c r="D51" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
         <v>15</v>
       </c>
       <c r="B52" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C52">
+        <v>4</v>
+      </c>
+      <c r="D52" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
         <v>15</v>
       </c>
       <c r="B53" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C53">
+        <v>3</v>
+      </c>
+      <c r="D53" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
         <v>15</v>
       </c>
       <c r="B54" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C54">
+        <v>5.5</v>
+      </c>
+      <c r="D54" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
         <v>15</v>
       </c>
       <c r="B55" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C55">
+        <v>0.75</v>
+      </c>
+      <c r="D55" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
         <v>17</v>
       </c>
       <c r="B56" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C56">
+        <v>0.9</v>
+      </c>
+      <c r="D56" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
         <v>17</v>
       </c>
       <c r="B57" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C57">
+        <v>1.2</v>
+      </c>
+      <c r="D57" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
         <v>17</v>
       </c>
       <c r="B58" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C58">
+        <v>1.5</v>
+      </c>
+      <c r="D58" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A59" t="s">
         <v>17</v>
       </c>
       <c r="B59" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C59">
+        <v>2.5</v>
+      </c>
+      <c r="D59" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A60" t="s">
         <v>17</v>
       </c>
       <c r="B60" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C60">
+        <v>4</v>
+      </c>
+      <c r="D60" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A61" t="s">
         <v>19</v>
       </c>
       <c r="B61" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C61">
+        <v>3</v>
+      </c>
+      <c r="D61" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A62" t="s">
         <v>19</v>
       </c>
       <c r="B62" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C62">
+        <v>5.5</v>
+      </c>
+      <c r="D62" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A63" t="s">
         <v>19</v>
       </c>
       <c r="B63" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C63">
+        <v>0.75</v>
+      </c>
+      <c r="D63" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A64" t="s">
         <v>19</v>
       </c>
       <c r="B64" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C64">
+        <v>0.9</v>
+      </c>
+      <c r="D64" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A65" t="s">
         <v>19</v>
       </c>
       <c r="B65" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C65">
+        <v>1.2</v>
+      </c>
+      <c r="D65" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
         <v>19</v>
       </c>
       <c r="B66" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C66">
+        <v>1.5</v>
+      </c>
+      <c r="D66" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
         <v>22</v>
       </c>
       <c r="B67" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C67">
+        <v>2.5</v>
+      </c>
+      <c r="D67" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A68" t="s">
         <v>22</v>
       </c>
       <c r="B68" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C68">
+        <v>4</v>
+      </c>
+      <c r="D68" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
         <v>22</v>
       </c>
       <c r="B69" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C69">
+        <v>3</v>
+      </c>
+      <c r="D69" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A70" t="s">
         <v>22</v>
       </c>
       <c r="B70" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C70">
+        <v>5.5</v>
+      </c>
+      <c r="D70" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A71" t="s">
         <v>22</v>
       </c>
       <c r="B71" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C71">
+        <v>0.75</v>
+      </c>
+      <c r="D71" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A72" t="s">
         <v>23</v>
       </c>
       <c r="B72" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C72">
+        <v>0.9</v>
+      </c>
+      <c r="D72" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A73" t="s">
         <v>23</v>
       </c>
       <c r="B73" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C73">
+        <v>1.2</v>
+      </c>
+      <c r="D73" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A74" t="s">
         <v>23</v>
       </c>
       <c r="B74" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C74">
+        <v>1.5</v>
+      </c>
+      <c r="D74" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A75" t="s">
         <v>23</v>
       </c>
       <c r="B75" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C75">
+        <v>2.5</v>
+      </c>
+      <c r="D75" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A76" t="s">
         <v>23</v>
       </c>
       <c r="B76" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C76">
+        <v>4</v>
+      </c>
+      <c r="D76" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A77" t="s">
         <v>25</v>
       </c>
       <c r="B77" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C77">
+        <v>3</v>
+      </c>
+      <c r="D77" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A78" t="s">
         <v>25</v>
       </c>
       <c r="B78" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C78">
+        <v>5.5</v>
+      </c>
+      <c r="D78" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A79" t="s">
         <v>25</v>
       </c>
       <c r="B79" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C79">
+        <v>0.75</v>
+      </c>
+      <c r="D79" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A80" t="s">
         <v>25</v>
       </c>
       <c r="B80" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C80">
+        <v>0.9</v>
+      </c>
+      <c r="D80" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A81" t="s">
         <v>25</v>
       </c>
       <c r="B81" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C81">
+        <v>1.2</v>
+      </c>
+      <c r="D81" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A82" t="s">
         <v>29</v>
       </c>
       <c r="B82" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C82">
+        <v>1.5</v>
+      </c>
+      <c r="D82" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A83" t="s">
         <v>29</v>
       </c>
       <c r="B83" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C83">
+        <v>2.5</v>
+      </c>
+      <c r="D83" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A84" t="s">
         <v>29</v>
       </c>
       <c r="B84" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C84">
+        <v>4</v>
+      </c>
+      <c r="D84" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A85" t="s">
         <v>29</v>
       </c>
       <c r="B85" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C85">
+        <v>3</v>
+      </c>
+      <c r="D85" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A86" t="s">
         <v>29</v>
       </c>
       <c r="B86" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C86">
+        <v>5.5</v>
+      </c>
+      <c r="D86" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A87" t="s">
         <v>30</v>
       </c>
       <c r="B87" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C87">
+        <v>0.75</v>
+      </c>
+      <c r="D87" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A88" t="s">
         <v>30</v>
       </c>
       <c r="B88" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C88">
+        <v>0.9</v>
+      </c>
+      <c r="D88" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A89" t="s">
         <v>30</v>
       </c>
       <c r="B89" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C89">
+        <v>1.2</v>
+      </c>
+      <c r="D89" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A90" t="s">
         <v>30</v>
       </c>
       <c r="B90" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C90">
+        <v>1.5</v>
+      </c>
+      <c r="D90" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A91" t="s">
         <v>30</v>
       </c>
       <c r="B91" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C91">
+        <v>2.5</v>
+      </c>
+      <c r="D91" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A92" t="s">
         <v>32</v>
       </c>
       <c r="B92" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C92">
+        <v>4</v>
+      </c>
+      <c r="D92" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A93" t="s">
         <v>32</v>
       </c>
       <c r="B93" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C93">
+        <v>3</v>
+      </c>
+      <c r="D93" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A94" t="s">
         <v>32</v>
       </c>
       <c r="B94" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C94">
+        <v>5.5</v>
+      </c>
+      <c r="D94" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A95" t="s">
         <v>32</v>
       </c>
       <c r="B95" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C95">
+        <v>0.75</v>
+      </c>
+      <c r="D95" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A96" t="s">
         <v>32</v>
       </c>
       <c r="B96" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C96">
+        <v>0.9</v>
+      </c>
+      <c r="D96" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A97" t="s">
         <v>33</v>
       </c>
       <c r="B97" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C97">
+        <v>1.2</v>
+      </c>
+      <c r="D97" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A98" t="s">
         <v>33</v>
       </c>
       <c r="B98" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C98">
+        <v>1.5</v>
+      </c>
+      <c r="D98" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A99" t="s">
         <v>33</v>
       </c>
       <c r="B99" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C99">
+        <v>2.5</v>
+      </c>
+      <c r="D99" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A100" t="s">
         <v>33</v>
       </c>
       <c r="B100" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C100">
+        <v>4</v>
+      </c>
+      <c r="D100" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A101" t="s">
         <v>33</v>
       </c>
       <c r="B101" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C101">
+        <v>3</v>
+      </c>
+      <c r="D101" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A102" t="s">
         <v>35</v>
       </c>
       <c r="B102" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C102">
+        <v>5.5</v>
+      </c>
+      <c r="D102" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A103" t="s">
         <v>35</v>
       </c>
       <c r="B103" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C103">
+        <v>0.75</v>
+      </c>
+      <c r="D103" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A104" t="s">
         <v>35</v>
       </c>
       <c r="B104" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C104">
+        <v>0.9</v>
+      </c>
+      <c r="D104" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A105" t="s">
         <v>35</v>
       </c>
       <c r="B105" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C105">
+        <v>1.2</v>
+      </c>
+      <c r="D105" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A106" t="s">
         <v>35</v>
       </c>
       <c r="B106" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C106">
+        <v>1.5</v>
+      </c>
+      <c r="D106" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A107" t="s">
         <v>40</v>
       </c>
       <c r="B107" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C107">
+        <v>2.5</v>
+      </c>
+      <c r="D107" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A108" t="s">
         <v>40</v>
       </c>
       <c r="B108" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C108">
+        <v>4</v>
+      </c>
+      <c r="D108" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A109" t="s">
         <v>40</v>
       </c>
       <c r="B109" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C109">
+        <v>3</v>
+      </c>
+      <c r="D109" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A110" t="s">
         <v>40</v>
       </c>
       <c r="B110" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C110">
+        <v>5.5</v>
+      </c>
+      <c r="D110" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A111" t="s">
         <v>40</v>
       </c>
       <c r="B111" t="s">
         <v>52</v>
+      </c>
+      <c r="C111">
+        <v>0.75</v>
+      </c>
+      <c r="D111" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2071,35 +2716,38 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{345B34B2-5EAF-4CBD-BC06-31035D0FFB87}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+        <v>109</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -2110,16 +2758,19 @@
         <v>50</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+        <v>101</v>
+      </c>
+      <c r="F2" s="5">
+        <v>18</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -2130,16 +2781,19 @@
         <v>50</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+        <v>102</v>
+      </c>
+      <c r="F3" s="5">
+        <v>18</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -2150,16 +2804,19 @@
         <v>50</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+        <v>103</v>
+      </c>
+      <c r="F4" s="5">
+        <v>18</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -2170,16 +2827,19 @@
         <v>50</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+        <v>101</v>
+      </c>
+      <c r="F5" s="5">
+        <v>18</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
@@ -2190,16 +2850,19 @@
         <v>50</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+        <v>102</v>
+      </c>
+      <c r="F6" s="5">
+        <v>18</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
@@ -2210,16 +2873,19 @@
         <v>50</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+        <v>103</v>
+      </c>
+      <c r="F7" s="5">
+        <v>18</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
@@ -2230,16 +2896,19 @@
         <v>50</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+        <v>101</v>
+      </c>
+      <c r="F8" s="5">
+        <v>75</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
         <v>15</v>
       </c>
@@ -2250,16 +2919,19 @@
         <v>50</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+        <v>102</v>
+      </c>
+      <c r="F9" s="5">
+        <v>75</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" s="5" t="s">
         <v>15</v>
       </c>
@@ -2270,16 +2942,19 @@
         <v>50</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+        <v>103</v>
+      </c>
+      <c r="F10" s="5">
+        <v>75</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
@@ -2290,16 +2965,19 @@
         <v>50</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+        <v>101</v>
+      </c>
+      <c r="F11" s="5">
+        <v>90</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" s="5" t="s">
         <v>15</v>
       </c>
@@ -2310,16 +2988,19 @@
         <v>50</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+        <v>102</v>
+      </c>
+      <c r="F12" s="5">
+        <v>90</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
@@ -2330,16 +3011,19 @@
         <v>50</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+        <v>103</v>
+      </c>
+      <c r="F13" s="5">
+        <v>90</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" s="5" t="s">
         <v>9</v>
       </c>
@@ -2350,16 +3034,19 @@
         <v>50</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+        <v>101</v>
+      </c>
+      <c r="F14" s="5">
+        <v>1000</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" s="5" t="s">
         <v>9</v>
       </c>
@@ -2370,16 +3057,19 @@
         <v>50</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+        <v>102</v>
+      </c>
+      <c r="F15" s="5">
+        <v>1000</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" s="5" t="s">
         <v>9</v>
       </c>
@@ -2390,16 +3080,19 @@
         <v>50</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+        <v>103</v>
+      </c>
+      <c r="F16" s="5">
+        <v>1000</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" s="5" t="s">
         <v>9</v>
       </c>
@@ -2410,16 +3103,19 @@
         <v>50</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+        <v>101</v>
+      </c>
+      <c r="F17" s="5">
+        <v>1000</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" s="5" t="s">
         <v>9</v>
       </c>
@@ -2430,16 +3126,19 @@
         <v>50</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+        <v>102</v>
+      </c>
+      <c r="F18" s="5">
+        <v>1000</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" s="5" t="s">
         <v>9</v>
       </c>
@@ -2450,16 +3149,19 @@
         <v>50</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+        <v>103</v>
+      </c>
+      <c r="F19" s="5">
+        <v>1000</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20" s="5" t="s">
         <v>19</v>
       </c>
@@ -2470,16 +3172,19 @@
         <v>50</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+        <v>101</v>
+      </c>
+      <c r="F20" s="5">
+        <v>46</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21" s="5" t="s">
         <v>19</v>
       </c>
@@ -2490,16 +3195,19 @@
         <v>50</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
+        <v>102</v>
+      </c>
+      <c r="F21" s="5">
+        <v>46</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A22" s="5" t="s">
         <v>19</v>
       </c>
@@ -2510,16 +3218,19 @@
         <v>50</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
+        <v>103</v>
+      </c>
+      <c r="F22" s="5">
+        <v>46</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A23" s="5" t="s">
         <v>19</v>
       </c>
@@ -2530,16 +3241,19 @@
         <v>50</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+        <v>101</v>
+      </c>
+      <c r="F23" s="5">
+        <v>56</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A24" s="5" t="s">
         <v>19</v>
       </c>
@@ -2550,16 +3264,19 @@
         <v>50</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+        <v>102</v>
+      </c>
+      <c r="F24" s="5">
+        <v>56</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A25" s="5" t="s">
         <v>19</v>
       </c>
@@ -2570,16 +3287,19 @@
         <v>50</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+        <v>103</v>
+      </c>
+      <c r="F25" s="5">
+        <v>56</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A26" s="5" t="s">
         <v>22</v>
       </c>
@@ -2590,16 +3310,19 @@
         <v>50</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
+        <v>101</v>
+      </c>
+      <c r="F26" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A27" s="5" t="s">
         <v>22</v>
       </c>
@@ -2610,16 +3333,19 @@
         <v>50</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
+        <v>102</v>
+      </c>
+      <c r="F27" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A28" s="5" t="s">
         <v>22</v>
       </c>
@@ -2630,16 +3356,19 @@
         <v>50</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
+        <v>103</v>
+      </c>
+      <c r="F28" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A29" s="5" t="s">
         <v>22</v>
       </c>
@@ -2650,16 +3379,19 @@
         <v>50</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
+        <v>101</v>
+      </c>
+      <c r="F29" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A30" s="5" t="s">
         <v>22</v>
       </c>
@@ -2670,16 +3402,19 @@
         <v>50</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
+        <v>102</v>
+      </c>
+      <c r="F30" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A31" s="5" t="s">
         <v>22</v>
       </c>
@@ -2690,16 +3425,19 @@
         <v>50</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
+        <v>103</v>
+      </c>
+      <c r="F31" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A32" s="5" t="s">
         <v>29</v>
       </c>
@@ -2710,16 +3448,19 @@
         <v>50</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
+        <v>101</v>
+      </c>
+      <c r="F32" s="5">
+        <v>25</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A33" s="5" t="s">
         <v>29</v>
       </c>
@@ -2730,16 +3471,19 @@
         <v>50</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
+        <v>102</v>
+      </c>
+      <c r="F33" s="5">
+        <v>25</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A34" s="5" t="s">
         <v>29</v>
       </c>
@@ -2750,16 +3494,19 @@
         <v>50</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
+        <v>103</v>
+      </c>
+      <c r="F34" s="5">
+        <v>25</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A35" s="5" t="s">
         <v>29</v>
       </c>
@@ -2770,16 +3517,19 @@
         <v>50</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
+        <v>101</v>
+      </c>
+      <c r="F35" s="5">
+        <v>30</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A36" s="5" t="s">
         <v>29</v>
       </c>
@@ -2790,16 +3540,19 @@
         <v>50</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
+        <v>102</v>
+      </c>
+      <c r="F36" s="5">
+        <v>30</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A37" s="5" t="s">
         <v>29</v>
       </c>
@@ -2810,13 +3563,16 @@
         <v>50</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>121</v>
+        <v>103</v>
+      </c>
+      <c r="F37" s="5">
+        <v>30</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new nutrient tree data
</commit_message>
<xml_diff>
--- a/nutrients.xlsx
+++ b/nutrients.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jyoth\Desktop\Project Expo\01. Nutri Master\05. Prototype\pdf_upload_website - v0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4875E003-87B3-4593-8F71-0C18D12EE8FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2017138C-ACF7-4B8E-9213-0808F948BB17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="8743" activeTab="2" xr2:uid="{7978047E-B5C9-4231-8CB2-CE9F13F7E962}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="8743" firstSheet="1" activeTab="2" xr2:uid="{7978047E-B5C9-4231-8CB2-CE9F13F7E962}"/>
   </bookViews>
   <sheets>
     <sheet name="food_nutrients_mapping" sheetId="3" r:id="rId1"/>
     <sheet name="nutrients_def_mapping" sheetId="2" r:id="rId2"/>
-    <sheet name="RDA" sheetId="4" r:id="rId3"/>
+    <sheet name="nutri_tree_dependencies" sheetId="5" r:id="rId3"/>
+    <sheet name="RDA" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="176">
   <si>
     <t>general_name</t>
   </si>
@@ -383,6 +384,189 @@
   </si>
   <si>
     <t>g</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Root</t>
+  </si>
+  <si>
+    <t>Indicator</t>
+  </si>
+  <si>
+    <t>Required</t>
+  </si>
+  <si>
+    <t>Micro</t>
+  </si>
+  <si>
+    <t>Enhances</t>
+  </si>
+  <si>
+    <t>Macro</t>
+  </si>
+  <si>
+    <t>Bone Health</t>
+  </si>
+  <si>
+    <t>Essential for oxygen transport</t>
+  </si>
+  <si>
+    <t>Fatigue, Weakness, Red Spots</t>
+  </si>
+  <si>
+    <t>Helps produce red blood cells</t>
+  </si>
+  <si>
+    <t>Pale skin, Weakness, Dizziness</t>
+  </si>
+  <si>
+    <t>Enhances iron absorption</t>
+  </si>
+  <si>
+    <t>Fatigue, Memory loss</t>
+  </si>
+  <si>
+    <t>Helps in red blood cell formation</t>
+  </si>
+  <si>
+    <t>Fatigue, Weakness, Memory loss</t>
+  </si>
+  <si>
+    <t>Fatigue, Weakness</t>
+  </si>
+  <si>
+    <t>Immune System</t>
+  </si>
+  <si>
+    <t>Supports immune function</t>
+  </si>
+  <si>
+    <t>Poor wound healing, Loss of taste</t>
+  </si>
+  <si>
+    <t>Works with zinc to promote immune function</t>
+  </si>
+  <si>
+    <t>Hair loss, Fatigue, Brain fog</t>
+  </si>
+  <si>
+    <t>Important for bone and muscle health</t>
+  </si>
+  <si>
+    <t>Muscle cramps, Weakness</t>
+  </si>
+  <si>
+    <t>Essential for strong bones</t>
+  </si>
+  <si>
+    <t>Brittle nails, Muscle spasms</t>
+  </si>
+  <si>
+    <t>Promotes calcium absorption</t>
+  </si>
+  <si>
+    <t>Bone pain, Muscle weakness</t>
+  </si>
+  <si>
+    <t>Works with calcium for bone mineralization</t>
+  </si>
+  <si>
+    <t>Easy bruising, Bleeding gums</t>
+  </si>
+  <si>
+    <t>Brain Function</t>
+  </si>
+  <si>
+    <t>Essential for brain and heart health</t>
+  </si>
+  <si>
+    <t>Memory issues, Dry skin</t>
+  </si>
+  <si>
+    <t>Omega-6</t>
+  </si>
+  <si>
+    <t>Works with Omega-3 for brain function</t>
+  </si>
+  <si>
+    <t>Hair loss, Dry skin</t>
+  </si>
+  <si>
+    <t>Iodine</t>
+  </si>
+  <si>
+    <t>Thyroid Health</t>
+  </si>
+  <si>
+    <t>Essential for thyroid hormone production</t>
+  </si>
+  <si>
+    <t>Weight gain, Swelling in neck</t>
+  </si>
+  <si>
+    <t>Muscle Function</t>
+  </si>
+  <si>
+    <t>Regulates fluid balance and muscle function</t>
+  </si>
+  <si>
+    <t>Muscle weakness, Constipation</t>
+  </si>
+  <si>
+    <t>Sodium</t>
+  </si>
+  <si>
+    <t>Works with potassium to balance fluids</t>
+  </si>
+  <si>
+    <t>Cramps, Low energy</t>
+  </si>
+  <si>
+    <t>Works with calcium for bone strength</t>
+  </si>
+  <si>
+    <t>Weakness, Bone pain</t>
+  </si>
+  <si>
+    <t>Vitamin A</t>
+  </si>
+  <si>
+    <t>Vision</t>
+  </si>
+  <si>
+    <t>Essential for vision and immune function</t>
+  </si>
+  <si>
+    <t>Night blindness, Dry eyes</t>
+  </si>
+  <si>
+    <t>Vitamin E</t>
+  </si>
+  <si>
+    <t>Skin Health</t>
+  </si>
+  <si>
+    <t>Works with Vitamin A to protect skin health</t>
+  </si>
+  <si>
+    <t>Dry skin, Vision problems</t>
+  </si>
+  <si>
+    <t>relation_type</t>
+  </si>
+  <si>
+    <t>depth</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>body_signs</t>
   </si>
 </sst>
 </file>
@@ -441,7 +625,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -457,6 +641,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2363,7 +2553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{247BE3D8-F4F2-4DB5-9A84-5A2CE70C7332}">
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -2715,11 +2905,518 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D52D8518-CCB2-47FA-9E07-B38A5D61EA2D}">
+  <dimension ref="A1:G21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="10.53515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.07421875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.84375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.69140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.921875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" s="7">
+        <v>0</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3" s="7">
+        <v>1</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" s="7">
+        <v>2</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" s="7">
+        <v>1</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D6" s="7">
+        <v>1</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7" s="7">
+        <v>2</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D8" s="7">
+        <v>1</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" s="7">
+        <v>2</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D10" s="7">
+        <v>1</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D11" s="7">
+        <v>1</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12" s="7">
+        <v>2</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13" s="7">
+        <v>2</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D14" s="7">
+        <v>1</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D15" s="7">
+        <v>1</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D16" s="7">
+        <v>1</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D17" s="7">
+        <v>1</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18" s="7">
+        <v>2</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D19" s="7">
+        <v>1</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D20" s="7">
+        <v>1</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21" s="7">
+        <v>2</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{345B34B2-5EAF-4CBD-BC06-31035D0FFB87}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
nutri tree updated data
</commit_message>
<xml_diff>
--- a/nutrients.xlsx
+++ b/nutrients.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jyoth\Desktop\Project Expo\01. Nutri Master\05. Prototype\pdf_upload_website - v0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB8F7EF1-BEB9-4800-9D77-182763534098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2031FBFA-1A41-4B85-99B1-BF0742812C5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="8743" firstSheet="1" activeTab="2" xr2:uid="{7978047E-B5C9-4231-8CB2-CE9F13F7E962}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="176">
   <si>
     <t>general_name</t>
   </si>
@@ -567,9 +567,6 @@
   </si>
   <si>
     <t>body_signs</t>
-  </si>
-  <si>
-    <t>parent_nutrient</t>
   </si>
 </sst>
 </file>
@@ -2912,7 +2909,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2931,7 +2928,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>176</v>
+        <v>0</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>171</v>

</xml_diff>